<commit_message>
Delete button disabled test - tabbed ui
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/CheckDeleteButtonDisabledRNAiHasEvidenceTest.xlsx
+++ b/src/main/resources/testdata/CheckDeleteButtonDisabledRNAiHasEvidenceTest.xlsx
@@ -4,15 +4,71 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="11055" windowHeight="3915"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="0"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+  <si>
+    <t>user</t>
+  </si>
+  <si>
+    <t>Data#</t>
+  </si>
+  <si>
+    <t>Test_Description</t>
+  </si>
+  <si>
+    <t>selectType</t>
+  </si>
+  <si>
+    <t>Genetic Feature</t>
+  </si>
+  <si>
+    <t>Check Delete Button disabled in tabbed view GF (GF with Evidence cannot be deleted)</t>
+  </si>
+  <si>
+    <t>Pillai, Nisha</t>
+  </si>
+  <si>
+    <t>search</t>
+  </si>
+  <si>
+    <t>Bharitkar S, Mendel</t>
+  </si>
+  <si>
+    <t>rationale</t>
+  </si>
+  <si>
+    <t>observation</t>
+  </si>
+  <si>
+    <t>enterText</t>
+  </si>
+  <si>
+    <t>trait</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>test observation</t>
+  </si>
+  <si>
+    <t>ath-MIR156a</t>
+  </si>
+  <si>
+    <t>biomass yield [en;XX;1]</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -46,7 +102,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -349,12 +406,83 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="79.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" customWidth="1"/>
+    <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>